<commit_message>
Install extension black for better coding presentation
</commit_message>
<xml_diff>
--- a/Driving/Driving.xlsx
+++ b/Driving/Driving.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Practice-Data-Science\Driving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314FD7D1-CFD8-41BB-AEE7-EAF80C1D5C08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067A9598-8871-4A5D-A8B2-049702889042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>App</t>
   </si>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,6 +1198,54 @@
         <v>827.16</v>
       </c>
     </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2">
+        <v>44360</v>
+      </c>
+      <c r="C17" s="1">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1">
+        <f>27*60</f>
+        <v>1620</v>
+      </c>
+      <c r="E17" s="1">
+        <f>30*60</f>
+        <v>1800</v>
+      </c>
+      <c r="F17" s="3">
+        <v>536.59</v>
+      </c>
+      <c r="G17" s="3">
+        <v>47.64</v>
+      </c>
+      <c r="H17" s="3">
+        <v>72.78</v>
+      </c>
+      <c r="I17" s="3">
+        <v>17.77</v>
+      </c>
+      <c r="J17" s="3">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="K17" s="3">
+        <v>255</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" ref="M17" si="2">SUM(F17:L17)</f>
+        <v>949.36</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" ref="N17" si="3">M17-J17</f>
+        <v>929.78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>